<commit_message>
[BE][TAIL-205] Chinese keywords and numeric words support (#196)
</commit_message>
<xml_diff>
--- a/common-lib/src/test/resources/matching/keywords.xlsx
+++ b/common-lib/src/test/resources/matching/keywords.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i829913/dev/kuaidao-svc/common-lib/src/test/resources/matching/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCCD3C5-DA7C-5D4A-853F-9E3C4EA3F503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA0DD86-2FDA-EB4D-AEF5-D80E3918E557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1440" uniqueCount="1307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1441" uniqueCount="1308">
   <si>
     <t>IT</t>
   </si>
@@ -4993,6 +4993,9 @@
   </si>
   <si>
     <t>市场调研</t>
+  </si>
+  <si>
+    <t>软件工程</t>
   </si>
 </sst>
 </file>
@@ -5383,7 +5386,7 @@
   <dimension ref="A1:AP93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8238,6 +8241,9 @@
       </c>
     </row>
     <row r="26" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>1307</v>
+      </c>
       <c r="C26" s="1" t="s">
         <v>235</v>
       </c>
@@ -9947,6 +9953,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007A9C639B6C5E334C96794AE379FAE9C3" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="136bf65708a02fa433f954ff8663f4f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ff398a5-2cbe-4d99-a5e5-de962d05c2cc" xmlns:ns3="2c39facb-0c33-4a8c-84bb-823165e11fb6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5829faac1f4637718733afa179ffc970" ns2:_="" ns3:_="">
     <xsd:import namespace="6ff398a5-2cbe-4d99-a5e5-de962d05c2cc"/>
@@ -10169,16 +10184,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <NFFormData xmlns="6ff398a5-2cbe-4d99-a5e5-de962d05c2cc" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormUrls xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms/url">
   <Display>FormsApp/NFLaunch.aspx?SPAppWebUrl=https://eyeshightc-f748fbd35587d3.sharepoint.com/sites/EyesHighTeamDrive/FormsApp&amp;SPHostUrl=https://eyeshightc.sharepoint.com/sites/EyesHighTeamDrive&amp;remoteAppUrl=https://formso365.nintex.com&amp;ctype=0x0101007A9C639B6C5E334C96794AE379FAE9C3&amp;wtg=/NintexFormXml/0x0101007A9C639B6C5E334C96794AE379FAE9C3_6ff398a5-2cbe-4d99-a5e5-de962d05c2cc/&amp;mode=2</Display>
@@ -10190,15 +10204,15 @@
 </FormUrls>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <NFFormData xmlns="6ff398a5-2cbe-4d99-a5e5-de962d05c2cc" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1BB062B-3F56-4582-9631-8C733322BACA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6CAA7073-B642-4974-AE2B-AE546DF9038C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10217,23 +10231,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1BB062B-3F56-4582-9631-8C733322BACA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33B67A10-6371-4ED0-9B22-DB02D035A57D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms/url"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2A9E3BA-9B6B-453E-8797-A4B4023252EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -10248,4 +10246,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33B67A10-6371-4ED0-9B22-DB02D035A57D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms/url"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>